<commit_message>
finished, access, admin, fabric, vmm, system
</commit_message>
<xml_diff>
--- a/Asgard_interface_selectors.xlsx
+++ b/Asgard_interface_selectors.xlsx
@@ -581,7 +581,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:D110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -649,7 +649,7 @@
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>vpc001</t>
+          <t>vpc0001</t>
         </is>
       </c>
       <c r="D3" s="2" t="n"/>
@@ -667,7 +667,7 @@
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t>vpc002</t>
+          <t>vpc0002</t>
         </is>
       </c>
       <c r="D4" s="1" t="n"/>
@@ -681,7 +681,7 @@
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>vpc003</t>
+          <t>vpc0003</t>
         </is>
       </c>
       <c r="D5" s="2" t="n"/>
@@ -695,7 +695,7 @@
       </c>
       <c r="C6" s="1" t="inlineStr">
         <is>
-          <t>vpc004</t>
+          <t>vpc0004</t>
         </is>
       </c>
       <c r="D6" s="1" t="n"/>
@@ -705,7 +705,7 @@
       <c r="B7" s="2" t="n"/>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>vpc005</t>
+          <t>vpc0005</t>
         </is>
       </c>
       <c r="D7" s="2" t="n"/>
@@ -715,7 +715,7 @@
       <c r="B8" s="1" t="n"/>
       <c r="C8" s="1" t="inlineStr">
         <is>
-          <t>vpc006</t>
+          <t>vpc0006</t>
         </is>
       </c>
       <c r="D8" s="1" t="n"/>
@@ -725,7 +725,7 @@
       <c r="B9" s="2" t="n"/>
       <c r="C9" s="2" t="inlineStr">
         <is>
-          <t>vpc007</t>
+          <t>vpc0007</t>
         </is>
       </c>
       <c r="D9" s="2" t="n"/>
@@ -735,7 +735,7 @@
       <c r="B10" s="1" t="n"/>
       <c r="C10" s="1" t="inlineStr">
         <is>
-          <t>vpc008</t>
+          <t>vpc0008</t>
         </is>
       </c>
       <c r="D10" s="1" t="n"/>
@@ -745,7 +745,7 @@
       <c r="B11" s="2" t="n"/>
       <c r="C11" s="2" t="inlineStr">
         <is>
-          <t>vpc009</t>
+          <t>vpc0009</t>
         </is>
       </c>
       <c r="D11" s="2" t="n"/>
@@ -755,7 +755,7 @@
       <c r="B12" s="1" t="n"/>
       <c r="C12" s="1" t="inlineStr">
         <is>
-          <t>vpc010</t>
+          <t>vpc0010</t>
         </is>
       </c>
       <c r="D12" s="1" t="n"/>
@@ -765,7 +765,7 @@
       <c r="B13" s="2" t="n"/>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>vpc011</t>
+          <t>vpc0011</t>
         </is>
       </c>
       <c r="D13" s="2" t="n"/>
@@ -775,7 +775,7 @@
       <c r="B14" s="1" t="n"/>
       <c r="C14" s="1" t="inlineStr">
         <is>
-          <t>vpc012</t>
+          <t>vpc0012</t>
         </is>
       </c>
       <c r="D14" s="1" t="n"/>
@@ -785,7 +785,7 @@
       <c r="B15" s="2" t="n"/>
       <c r="C15" s="2" t="inlineStr">
         <is>
-          <t>vpc013</t>
+          <t>vpc0013</t>
         </is>
       </c>
       <c r="D15" s="2" t="n"/>
@@ -795,7 +795,7 @@
       <c r="B16" s="1" t="n"/>
       <c r="C16" s="1" t="inlineStr">
         <is>
-          <t>vpc014</t>
+          <t>vpc0014</t>
         </is>
       </c>
       <c r="D16" s="1" t="n"/>
@@ -805,7 +805,7 @@
       <c r="B17" s="2" t="n"/>
       <c r="C17" s="2" t="inlineStr">
         <is>
-          <t>vpc015</t>
+          <t>vpc0015</t>
         </is>
       </c>
       <c r="D17" s="2" t="n"/>
@@ -815,7 +815,7 @@
       <c r="B18" s="1" t="n"/>
       <c r="C18" s="1" t="inlineStr">
         <is>
-          <t>vpc016</t>
+          <t>vpc0016</t>
         </is>
       </c>
       <c r="D18" s="1" t="n"/>
@@ -825,7 +825,7 @@
       <c r="B19" s="2" t="n"/>
       <c r="C19" s="2" t="inlineStr">
         <is>
-          <t>vpc017</t>
+          <t>vpc0017</t>
         </is>
       </c>
       <c r="D19" s="2" t="n"/>
@@ -835,7 +835,7 @@
       <c r="B20" s="1" t="n"/>
       <c r="C20" s="1" t="inlineStr">
         <is>
-          <t>vpc018</t>
+          <t>vpc0018</t>
         </is>
       </c>
       <c r="D20" s="1" t="n"/>
@@ -845,7 +845,7 @@
       <c r="B21" s="2" t="n"/>
       <c r="C21" s="2" t="inlineStr">
         <is>
-          <t>vpc019</t>
+          <t>vpc0019</t>
         </is>
       </c>
       <c r="D21" s="2" t="n"/>
@@ -855,7 +855,7 @@
       <c r="B22" s="1" t="n"/>
       <c r="C22" s="1" t="inlineStr">
         <is>
-          <t>vpc020</t>
+          <t>vpc0020</t>
         </is>
       </c>
       <c r="D22" s="1" t="n"/>
@@ -865,7 +865,7 @@
       <c r="B23" s="2" t="n"/>
       <c r="C23" s="2" t="inlineStr">
         <is>
-          <t>vpc021</t>
+          <t>vpc0021</t>
         </is>
       </c>
       <c r="D23" s="2" t="n"/>
@@ -875,7 +875,7 @@
       <c r="B24" s="1" t="n"/>
       <c r="C24" s="1" t="inlineStr">
         <is>
-          <t>vpc022</t>
+          <t>vpc0022</t>
         </is>
       </c>
       <c r="D24" s="1" t="n"/>
@@ -885,7 +885,7 @@
       <c r="B25" s="2" t="n"/>
       <c r="C25" s="2" t="inlineStr">
         <is>
-          <t>vpc023</t>
+          <t>vpc0023</t>
         </is>
       </c>
       <c r="D25" s="2" t="n"/>
@@ -895,7 +895,7 @@
       <c r="B26" s="1" t="n"/>
       <c r="C26" s="1" t="inlineStr">
         <is>
-          <t>vpc024</t>
+          <t>vpc0024</t>
         </is>
       </c>
       <c r="D26" s="1" t="n"/>
@@ -905,7 +905,7 @@
       <c r="B27" s="2" t="n"/>
       <c r="C27" s="2" t="inlineStr">
         <is>
-          <t>vpc025</t>
+          <t>vpc0025</t>
         </is>
       </c>
       <c r="D27" s="2" t="n"/>
@@ -915,7 +915,7 @@
       <c r="B28" s="1" t="n"/>
       <c r="C28" s="1" t="inlineStr">
         <is>
-          <t>vpc026</t>
+          <t>vpc0026</t>
         </is>
       </c>
       <c r="D28" s="1" t="n"/>
@@ -925,7 +925,7 @@
       <c r="B29" s="2" t="n"/>
       <c r="C29" s="2" t="inlineStr">
         <is>
-          <t>vpc027</t>
+          <t>vpc0027</t>
         </is>
       </c>
       <c r="D29" s="2" t="n"/>
@@ -935,7 +935,7 @@
       <c r="B30" s="1" t="n"/>
       <c r="C30" s="1" t="inlineStr">
         <is>
-          <t>vpc028</t>
+          <t>vpc0028</t>
         </is>
       </c>
       <c r="D30" s="1" t="n"/>
@@ -945,7 +945,7 @@
       <c r="B31" s="2" t="n"/>
       <c r="C31" s="2" t="inlineStr">
         <is>
-          <t>vpc029</t>
+          <t>vpc0029</t>
         </is>
       </c>
       <c r="D31" s="2" t="n"/>
@@ -955,7 +955,7 @@
       <c r="B32" s="1" t="n"/>
       <c r="C32" s="1" t="inlineStr">
         <is>
-          <t>vpc030</t>
+          <t>vpc0030</t>
         </is>
       </c>
       <c r="D32" s="1" t="n"/>
@@ -965,7 +965,7 @@
       <c r="B33" s="2" t="n"/>
       <c r="C33" s="2" t="inlineStr">
         <is>
-          <t>vpc031</t>
+          <t>vpc0031</t>
         </is>
       </c>
       <c r="D33" s="2" t="n"/>
@@ -975,7 +975,7 @@
       <c r="B34" s="1" t="n"/>
       <c r="C34" s="1" t="inlineStr">
         <is>
-          <t>vpc032</t>
+          <t>vpc0032</t>
         </is>
       </c>
       <c r="D34" s="1" t="n"/>
@@ -985,7 +985,7 @@
       <c r="B35" s="2" t="n"/>
       <c r="C35" s="2" t="inlineStr">
         <is>
-          <t>vpc033</t>
+          <t>vpc0033</t>
         </is>
       </c>
       <c r="D35" s="2" t="n"/>
@@ -995,7 +995,7 @@
       <c r="B36" s="1" t="n"/>
       <c r="C36" s="1" t="inlineStr">
         <is>
-          <t>vpc034</t>
+          <t>vpc0034</t>
         </is>
       </c>
       <c r="D36" s="1" t="n"/>
@@ -1005,7 +1005,7 @@
       <c r="B37" s="2" t="n"/>
       <c r="C37" s="2" t="inlineStr">
         <is>
-          <t>vpc035</t>
+          <t>vpc0035</t>
         </is>
       </c>
       <c r="D37" s="2" t="n"/>
@@ -1015,7 +1015,7 @@
       <c r="B38" s="1" t="n"/>
       <c r="C38" s="1" t="inlineStr">
         <is>
-          <t>vpc036</t>
+          <t>vpc0036</t>
         </is>
       </c>
       <c r="D38" s="1" t="n"/>
@@ -1025,7 +1025,7 @@
       <c r="B39" s="2" t="n"/>
       <c r="C39" s="2" t="inlineStr">
         <is>
-          <t>vpc037</t>
+          <t>vpc0037</t>
         </is>
       </c>
       <c r="D39" s="2" t="n"/>
@@ -1035,7 +1035,7 @@
       <c r="B40" s="1" t="n"/>
       <c r="C40" s="1" t="inlineStr">
         <is>
-          <t>vpc038</t>
+          <t>vpc0038</t>
         </is>
       </c>
       <c r="D40" s="1" t="n"/>
@@ -1045,7 +1045,7 @@
       <c r="B41" s="2" t="n"/>
       <c r="C41" s="2" t="inlineStr">
         <is>
-          <t>vpc039</t>
+          <t>vpc0039</t>
         </is>
       </c>
       <c r="D41" s="2" t="n"/>
@@ -1055,7 +1055,7 @@
       <c r="B42" s="1" t="n"/>
       <c r="C42" s="1" t="inlineStr">
         <is>
-          <t>vpc040</t>
+          <t>vpc0040</t>
         </is>
       </c>
       <c r="D42" s="1" t="n"/>
@@ -1065,7 +1065,7 @@
       <c r="B43" s="2" t="n"/>
       <c r="C43" s="2" t="inlineStr">
         <is>
-          <t>vpc041</t>
+          <t>vpc0041</t>
         </is>
       </c>
       <c r="D43" s="2" t="n"/>
@@ -1075,7 +1075,7 @@
       <c r="B44" s="1" t="n"/>
       <c r="C44" s="1" t="inlineStr">
         <is>
-          <t>vpc042</t>
+          <t>vpc0042</t>
         </is>
       </c>
       <c r="D44" s="1" t="n"/>
@@ -1085,7 +1085,7 @@
       <c r="B45" s="2" t="n"/>
       <c r="C45" s="2" t="inlineStr">
         <is>
-          <t>vpc043</t>
+          <t>vpc0043</t>
         </is>
       </c>
       <c r="D45" s="2" t="n"/>
@@ -1095,7 +1095,7 @@
       <c r="B46" s="1" t="n"/>
       <c r="C46" s="1" t="inlineStr">
         <is>
-          <t>vpc044</t>
+          <t>vpc0044</t>
         </is>
       </c>
       <c r="D46" s="1" t="n"/>
@@ -1105,7 +1105,7 @@
       <c r="B47" s="2" t="n"/>
       <c r="C47" s="2" t="inlineStr">
         <is>
-          <t>vpc045</t>
+          <t>vpc0045</t>
         </is>
       </c>
       <c r="D47" s="2" t="n"/>
@@ -1115,7 +1115,7 @@
       <c r="B48" s="1" t="n"/>
       <c r="C48" s="1" t="inlineStr">
         <is>
-          <t>vpc046</t>
+          <t>vpc0046</t>
         </is>
       </c>
       <c r="D48" s="1" t="n"/>
@@ -1125,7 +1125,7 @@
       <c r="B49" s="2" t="n"/>
       <c r="C49" s="2" t="inlineStr">
         <is>
-          <t>vpc047</t>
+          <t>vpc0047</t>
         </is>
       </c>
       <c r="D49" s="2" t="n"/>
@@ -1135,7 +1135,7 @@
       <c r="B50" s="1" t="n"/>
       <c r="C50" s="1" t="inlineStr">
         <is>
-          <t>vpc048</t>
+          <t>vpc0048</t>
         </is>
       </c>
       <c r="D50" s="1" t="n"/>
@@ -1145,7 +1145,7 @@
       <c r="B51" s="2" t="n"/>
       <c r="C51" s="2" t="inlineStr">
         <is>
-          <t>vpc049</t>
+          <t>vpc0049</t>
         </is>
       </c>
       <c r="D51" s="2" t="n"/>
@@ -1155,7 +1155,7 @@
       <c r="B52" s="1" t="n"/>
       <c r="C52" s="1" t="inlineStr">
         <is>
-          <t>vpc050</t>
+          <t>vpc0050</t>
         </is>
       </c>
       <c r="D52" s="1" t="n"/>
@@ -1165,7 +1165,7 @@
       <c r="B53" s="2" t="n"/>
       <c r="C53" s="2" t="inlineStr">
         <is>
-          <t>vpc051</t>
+          <t>vpc0051</t>
         </is>
       </c>
       <c r="D53" s="2" t="n"/>
@@ -1175,7 +1175,7 @@
       <c r="B54" s="1" t="n"/>
       <c r="C54" s="1" t="inlineStr">
         <is>
-          <t>vpc052</t>
+          <t>vpc0052</t>
         </is>
       </c>
       <c r="D54" s="1" t="n"/>
@@ -1185,7 +1185,7 @@
       <c r="B55" s="2" t="n"/>
       <c r="C55" s="2" t="inlineStr">
         <is>
-          <t>vpc053</t>
+          <t>vpc0053</t>
         </is>
       </c>
       <c r="D55" s="2" t="n"/>
@@ -1195,7 +1195,7 @@
       <c r="B56" s="1" t="n"/>
       <c r="C56" s="1" t="inlineStr">
         <is>
-          <t>vpc054</t>
+          <t>vpc0054</t>
         </is>
       </c>
       <c r="D56" s="1" t="n"/>
@@ -1205,7 +1205,7 @@
       <c r="B57" s="2" t="n"/>
       <c r="C57" s="2" t="inlineStr">
         <is>
-          <t>vpc055</t>
+          <t>vpc0055</t>
         </is>
       </c>
       <c r="D57" s="2" t="n"/>
@@ -1215,7 +1215,7 @@
       <c r="B58" s="1" t="n"/>
       <c r="C58" s="1" t="inlineStr">
         <is>
-          <t>vpc056</t>
+          <t>vpc0056</t>
         </is>
       </c>
       <c r="D58" s="1" t="n"/>
@@ -1225,7 +1225,7 @@
       <c r="B59" s="2" t="n"/>
       <c r="C59" s="2" t="inlineStr">
         <is>
-          <t>vpc057</t>
+          <t>vpc0057</t>
         </is>
       </c>
       <c r="D59" s="2" t="n"/>
@@ -1235,7 +1235,7 @@
       <c r="B60" s="1" t="n"/>
       <c r="C60" s="1" t="inlineStr">
         <is>
-          <t>vpc058</t>
+          <t>vpc0058</t>
         </is>
       </c>
       <c r="D60" s="1" t="n"/>
@@ -1245,7 +1245,7 @@
       <c r="B61" s="2" t="n"/>
       <c r="C61" s="2" t="inlineStr">
         <is>
-          <t>vpc059</t>
+          <t>vpc0059</t>
         </is>
       </c>
       <c r="D61" s="2" t="n"/>
@@ -1255,10 +1255,490 @@
       <c r="B62" s="1" t="n"/>
       <c r="C62" s="1" t="inlineStr">
         <is>
-          <t>vpc060</t>
+          <t>vpc0060</t>
         </is>
       </c>
       <c r="D62" s="1" t="n"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="2" t="n"/>
+      <c r="B63" s="2" t="n"/>
+      <c r="C63" s="2" t="inlineStr">
+        <is>
+          <t>vpc0061</t>
+        </is>
+      </c>
+      <c r="D63" s="2" t="n"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n"/>
+      <c r="B64" s="1" t="n"/>
+      <c r="C64" s="1" t="inlineStr">
+        <is>
+          <t>vpc0062</t>
+        </is>
+      </c>
+      <c r="D64" s="1" t="n"/>
+    </row>
+    <row r="65">
+      <c r="A65" s="2" t="n"/>
+      <c r="B65" s="2" t="n"/>
+      <c r="C65" s="2" t="inlineStr">
+        <is>
+          <t>vpc0063</t>
+        </is>
+      </c>
+      <c r="D65" s="2" t="n"/>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n"/>
+      <c r="B66" s="1" t="n"/>
+      <c r="C66" s="1" t="inlineStr">
+        <is>
+          <t>vpc0064</t>
+        </is>
+      </c>
+      <c r="D66" s="1" t="n"/>
+    </row>
+    <row r="67">
+      <c r="A67" s="2" t="n"/>
+      <c r="B67" s="2" t="n"/>
+      <c r="C67" s="2" t="inlineStr">
+        <is>
+          <t>vpc0065</t>
+        </is>
+      </c>
+      <c r="D67" s="2" t="n"/>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n"/>
+      <c r="B68" s="1" t="n"/>
+      <c r="C68" s="1" t="inlineStr">
+        <is>
+          <t>vpc0066</t>
+        </is>
+      </c>
+      <c r="D68" s="1" t="n"/>
+    </row>
+    <row r="69">
+      <c r="A69" s="2" t="n"/>
+      <c r="B69" s="2" t="n"/>
+      <c r="C69" s="2" t="inlineStr">
+        <is>
+          <t>vpc0067</t>
+        </is>
+      </c>
+      <c r="D69" s="2" t="n"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n"/>
+      <c r="B70" s="1" t="n"/>
+      <c r="C70" s="1" t="inlineStr">
+        <is>
+          <t>vpc0068</t>
+        </is>
+      </c>
+      <c r="D70" s="1" t="n"/>
+    </row>
+    <row r="71">
+      <c r="A71" s="2" t="n"/>
+      <c r="B71" s="2" t="n"/>
+      <c r="C71" s="2" t="inlineStr">
+        <is>
+          <t>vpc0069</t>
+        </is>
+      </c>
+      <c r="D71" s="2" t="n"/>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n"/>
+      <c r="B72" s="1" t="n"/>
+      <c r="C72" s="1" t="inlineStr">
+        <is>
+          <t>vpc0070</t>
+        </is>
+      </c>
+      <c r="D72" s="1" t="n"/>
+    </row>
+    <row r="73">
+      <c r="A73" s="2" t="n"/>
+      <c r="B73" s="2" t="n"/>
+      <c r="C73" s="2" t="inlineStr">
+        <is>
+          <t>vpc0071</t>
+        </is>
+      </c>
+      <c r="D73" s="2" t="n"/>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n"/>
+      <c r="B74" s="1" t="n"/>
+      <c r="C74" s="1" t="inlineStr">
+        <is>
+          <t>vpc0072</t>
+        </is>
+      </c>
+      <c r="D74" s="1" t="n"/>
+    </row>
+    <row r="75">
+      <c r="A75" s="2" t="n"/>
+      <c r="B75" s="2" t="n"/>
+      <c r="C75" s="2" t="inlineStr">
+        <is>
+          <t>vpc0073</t>
+        </is>
+      </c>
+      <c r="D75" s="2" t="n"/>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n"/>
+      <c r="B76" s="1" t="n"/>
+      <c r="C76" s="1" t="inlineStr">
+        <is>
+          <t>vpc0074</t>
+        </is>
+      </c>
+      <c r="D76" s="1" t="n"/>
+    </row>
+    <row r="77">
+      <c r="A77" s="2" t="n"/>
+      <c r="B77" s="2" t="n"/>
+      <c r="C77" s="2" t="inlineStr">
+        <is>
+          <t>vpc0075</t>
+        </is>
+      </c>
+      <c r="D77" s="2" t="n"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n"/>
+      <c r="B78" s="1" t="n"/>
+      <c r="C78" s="1" t="inlineStr">
+        <is>
+          <t>vpc0076</t>
+        </is>
+      </c>
+      <c r="D78" s="1" t="n"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="2" t="n"/>
+      <c r="B79" s="2" t="n"/>
+      <c r="C79" s="2" t="inlineStr">
+        <is>
+          <t>vpc0077</t>
+        </is>
+      </c>
+      <c r="D79" s="2" t="n"/>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n"/>
+      <c r="B80" s="1" t="n"/>
+      <c r="C80" s="1" t="inlineStr">
+        <is>
+          <t>vpc0078</t>
+        </is>
+      </c>
+      <c r="D80" s="1" t="n"/>
+    </row>
+    <row r="81">
+      <c r="A81" s="2" t="n"/>
+      <c r="B81" s="2" t="n"/>
+      <c r="C81" s="2" t="inlineStr">
+        <is>
+          <t>vpc0079</t>
+        </is>
+      </c>
+      <c r="D81" s="2" t="n"/>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n"/>
+      <c r="B82" s="1" t="n"/>
+      <c r="C82" s="1" t="inlineStr">
+        <is>
+          <t>vpc0080</t>
+        </is>
+      </c>
+      <c r="D82" s="1" t="n"/>
+    </row>
+    <row r="83">
+      <c r="A83" s="2" t="n"/>
+      <c r="B83" s="2" t="n"/>
+      <c r="C83" s="2" t="inlineStr">
+        <is>
+          <t>vpc0081</t>
+        </is>
+      </c>
+      <c r="D83" s="2" t="n"/>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n"/>
+      <c r="B84" s="1" t="n"/>
+      <c r="C84" s="1" t="inlineStr">
+        <is>
+          <t>vpc0082</t>
+        </is>
+      </c>
+      <c r="D84" s="1" t="n"/>
+    </row>
+    <row r="85">
+      <c r="A85" s="2" t="n"/>
+      <c r="B85" s="2" t="n"/>
+      <c r="C85" s="2" t="inlineStr">
+        <is>
+          <t>vpc0083</t>
+        </is>
+      </c>
+      <c r="D85" s="2" t="n"/>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n"/>
+      <c r="B86" s="1" t="n"/>
+      <c r="C86" s="1" t="inlineStr">
+        <is>
+          <t>vpc0084</t>
+        </is>
+      </c>
+      <c r="D86" s="1" t="n"/>
+    </row>
+    <row r="87">
+      <c r="A87" s="2" t="n"/>
+      <c r="B87" s="2" t="n"/>
+      <c r="C87" s="2" t="inlineStr">
+        <is>
+          <t>vpc0085</t>
+        </is>
+      </c>
+      <c r="D87" s="2" t="n"/>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="n"/>
+      <c r="B88" s="1" t="n"/>
+      <c r="C88" s="1" t="inlineStr">
+        <is>
+          <t>vpc0086</t>
+        </is>
+      </c>
+      <c r="D88" s="1" t="n"/>
+    </row>
+    <row r="89">
+      <c r="A89" s="2" t="n"/>
+      <c r="B89" s="2" t="n"/>
+      <c r="C89" s="2" t="inlineStr">
+        <is>
+          <t>vpc0087</t>
+        </is>
+      </c>
+      <c r="D89" s="2" t="n"/>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="n"/>
+      <c r="B90" s="1" t="n"/>
+      <c r="C90" s="1" t="inlineStr">
+        <is>
+          <t>vpc0088</t>
+        </is>
+      </c>
+      <c r="D90" s="1" t="n"/>
+    </row>
+    <row r="91">
+      <c r="A91" s="2" t="n"/>
+      <c r="B91" s="2" t="n"/>
+      <c r="C91" s="2" t="inlineStr">
+        <is>
+          <t>vpc0089</t>
+        </is>
+      </c>
+      <c r="D91" s="2" t="n"/>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="n"/>
+      <c r="B92" s="1" t="n"/>
+      <c r="C92" s="1" t="inlineStr">
+        <is>
+          <t>vpc0090</t>
+        </is>
+      </c>
+      <c r="D92" s="1" t="n"/>
+    </row>
+    <row r="93">
+      <c r="A93" s="2" t="n"/>
+      <c r="B93" s="2" t="n"/>
+      <c r="C93" s="2" t="inlineStr">
+        <is>
+          <t>vpc0091</t>
+        </is>
+      </c>
+      <c r="D93" s="2" t="n"/>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="n"/>
+      <c r="B94" s="1" t="n"/>
+      <c r="C94" s="1" t="inlineStr">
+        <is>
+          <t>vpc0092</t>
+        </is>
+      </c>
+      <c r="D94" s="1" t="n"/>
+    </row>
+    <row r="95">
+      <c r="A95" s="2" t="n"/>
+      <c r="B95" s="2" t="n"/>
+      <c r="C95" s="2" t="inlineStr">
+        <is>
+          <t>vpc0093</t>
+        </is>
+      </c>
+      <c r="D95" s="2" t="n"/>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="n"/>
+      <c r="B96" s="1" t="n"/>
+      <c r="C96" s="1" t="inlineStr">
+        <is>
+          <t>vpc0094</t>
+        </is>
+      </c>
+      <c r="D96" s="1" t="n"/>
+    </row>
+    <row r="97">
+      <c r="A97" s="2" t="n"/>
+      <c r="B97" s="2" t="n"/>
+      <c r="C97" s="2" t="inlineStr">
+        <is>
+          <t>vpc0095</t>
+        </is>
+      </c>
+      <c r="D97" s="2" t="n"/>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n"/>
+      <c r="B98" s="1" t="n"/>
+      <c r="C98" s="1" t="inlineStr">
+        <is>
+          <t>vpc0096</t>
+        </is>
+      </c>
+      <c r="D98" s="1" t="n"/>
+    </row>
+    <row r="99">
+      <c r="A99" s="2" t="n"/>
+      <c r="B99" s="2" t="n"/>
+      <c r="C99" s="2" t="inlineStr">
+        <is>
+          <t>vpc0097</t>
+        </is>
+      </c>
+      <c r="D99" s="2" t="n"/>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n"/>
+      <c r="B100" s="1" t="n"/>
+      <c r="C100" s="1" t="inlineStr">
+        <is>
+          <t>vpc0098</t>
+        </is>
+      </c>
+      <c r="D100" s="1" t="n"/>
+    </row>
+    <row r="101">
+      <c r="A101" s="2" t="n"/>
+      <c r="B101" s="2" t="n"/>
+      <c r="C101" s="2" t="inlineStr">
+        <is>
+          <t>vpc0099</t>
+        </is>
+      </c>
+      <c r="D101" s="2" t="n"/>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="n"/>
+      <c r="B102" s="1" t="n"/>
+      <c r="C102" s="1" t="inlineStr">
+        <is>
+          <t>vpc0100</t>
+        </is>
+      </c>
+      <c r="D102" s="1" t="n"/>
+    </row>
+    <row r="103">
+      <c r="A103" s="2" t="n"/>
+      <c r="B103" s="2" t="n"/>
+      <c r="C103" s="2" t="inlineStr">
+        <is>
+          <t>vpc0101</t>
+        </is>
+      </c>
+      <c r="D103" s="2" t="n"/>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="n"/>
+      <c r="B104" s="1" t="n"/>
+      <c r="C104" s="1" t="inlineStr">
+        <is>
+          <t>vpc0102</t>
+        </is>
+      </c>
+      <c r="D104" s="1" t="n"/>
+    </row>
+    <row r="105">
+      <c r="A105" s="2" t="n"/>
+      <c r="B105" s="2" t="n"/>
+      <c r="C105" s="2" t="inlineStr">
+        <is>
+          <t>vpc0103</t>
+        </is>
+      </c>
+      <c r="D105" s="2" t="n"/>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n"/>
+      <c r="B106" s="1" t="n"/>
+      <c r="C106" s="1" t="inlineStr">
+        <is>
+          <t>vpc0104</t>
+        </is>
+      </c>
+      <c r="D106" s="1" t="n"/>
+    </row>
+    <row r="107">
+      <c r="A107" s="2" t="n"/>
+      <c r="B107" s="2" t="n"/>
+      <c r="C107" s="2" t="inlineStr">
+        <is>
+          <t>vpc0105</t>
+        </is>
+      </c>
+      <c r="D107" s="2" t="n"/>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="n"/>
+      <c r="B108" s="1" t="n"/>
+      <c r="C108" s="1" t="inlineStr">
+        <is>
+          <t>vpc0106</t>
+        </is>
+      </c>
+      <c r="D108" s="1" t="n"/>
+    </row>
+    <row r="109">
+      <c r="A109" s="2" t="n"/>
+      <c r="B109" s="2" t="n"/>
+      <c r="C109" s="2" t="inlineStr">
+        <is>
+          <t>vpc0107</t>
+        </is>
+      </c>
+      <c r="D109" s="2" t="n"/>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="n"/>
+      <c r="B110" s="1" t="n"/>
+      <c r="C110" s="1" t="inlineStr">
+        <is>
+          <t>vpc0108</t>
+        </is>
+      </c>
+      <c r="D110" s="1" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>